<commit_message>
Adiciona solucao final para 2023.2
</commit_message>
<xml_diff>
--- a/dados/salas_preferenciais_2023.1.xlsx
+++ b/dados/salas_preferenciais_2023.1.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">ADMINISTRAÇÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">206-B,207-B,208-B,209-B,103-C</t>
+    <t xml:space="preserve">206-B,207-B,208-B,209-B,312-C</t>
   </si>
   <si>
     <t xml:space="preserve">Preferências de matéria sobrescrevem as preferencias de curso</t>
@@ -43,23 +43,7 @@
     <t xml:space="preserve">AGRONOMIA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">201-B,302-B,303-B,304-B,305-B,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">103-C</t>
-    </r>
+    <t xml:space="preserve">201-B,302-B,303-B,304-B,305-B,105-C</t>
   </si>
   <si>
     <t xml:space="preserve">Separar as salas por “,”</t>
@@ -68,23 +52,7 @@
     <t xml:space="preserve">CIÊNCIA DA COMPUTAÇÃO</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">305-B,308-B,309-B,310-B,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">103-C,217-C,302-C</t>
-    </r>
+    <t xml:space="preserve">305-B,308-B,309-B,310-B,313-C</t>
   </si>
   <si>
     <t xml:space="preserve">Atenção para o formato da identificação das salas {número}-{bloco}</t>
@@ -93,32 +61,46 @@
     <t xml:space="preserve">CIÊNCIAS SOCIAIS</t>
   </si>
   <si>
-    <t xml:space="preserve">302-A,303-A,309-A,216-C</t>
+    <t xml:space="preserve">201-A,302-A,303-A,309-A,302-C</t>
   </si>
   <si>
     <t xml:space="preserve">ENFERMAGEM</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">301-A,305-A,307-A,308-A,309-A,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">103-C,215-C</t>
-    </r>
+    <t xml:space="preserve">301-A,305-A,307-A,308-A,309-A,105-C</t>
   </si>
   <si>
     <t xml:space="preserve">ENGENHARIA AMBIENTAL E SANITÁRIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201-A,202-A,203-A,204-A,205-A,302-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FILOSOFIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301-A,304-A,301-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEOGRAFIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301-B,302-B,303-B,313-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HISTÓRIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">305-A,306-A,307-A,308-A,313-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LETRAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">206-A,207-A,208-A,209-A,220-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATEMÁTICA</t>
   </si>
   <si>
     <r>
@@ -136,82 +118,20 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">216-C</t>
+      <t xml:space="preserve">312-C</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">FILOSOFIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">301-A,304-A,215-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEOGRAFIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">301-B,302-B,303-B,302-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HISTÓRIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">305-A,306-A,307-A,308-A,217-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LETRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">206-A,207-A,208-A,209-A,105-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATEMÁTICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201-A,202-A,203-A,204-A,205-A</t>
-  </si>
-  <si>
     <t xml:space="preserve">MEDICINA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">303-A,304-A,309-B,310-B,208-B,209-B,301-B,302-B,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">103-C</t>
-    </r>
+    <t xml:space="preserve">303-A,304-A,309-B,310-B,208-B,209-B,301-B,302-B</t>
   </si>
   <si>
     <t xml:space="preserve">PEDAGOGIA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">201-B,202-B,203-B,204-B,205-B,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">302-C</t>
-    </r>
+    <t xml:space="preserve">201-B,202-B,203-B,204-B,205-B,313-C</t>
   </si>
 </sst>
 </file>
@@ -348,10 +268,10 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="101.86"/>

</xml_diff>